<commit_message>
feat: add more prompt tests
</commit_message>
<xml_diff>
--- a/Quiz_Analysis_Gemini_Prompts.xlsx
+++ b/Quiz_Analysis_Gemini_Prompts.xlsx
@@ -543,26 +543,26 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>verbose</t>
+          <t>blooms_taxonomy</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2" t="n">
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="G2" t="n">
-        <v>27.09</v>
+        <v>35.88</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -571,40 +571,40 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>7.681</v>
+        <v>3.683</v>
       </c>
       <c r="K2" t="n">
-        <v>0.213</v>
+        <v>0.198</v>
       </c>
       <c r="L2" t="n">
-        <v>20</v>
+        <v>33.33</v>
       </c>
       <c r="M2" t="n">
-        <v>10</v>
+        <v>6.67</v>
       </c>
       <c r="N2" t="n">
         <v>100</v>
       </c>
       <c r="O2" t="n">
-        <v>60</v>
+        <v>46.67</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>0.53</v>
       </c>
       <c r="Q2" t="n">
-        <v>70</v>
+        <v>37.78</v>
       </c>
       <c r="R2" t="n">
-        <v>0.0141</v>
+        <v>0.0145</v>
       </c>
       <c r="S2" t="n">
-        <v>30</v>
+        <v>17.78</v>
       </c>
       <c r="T2" t="n">
-        <v>0.743</v>
+        <v>0.783</v>
       </c>
       <c r="U2" t="n">
-        <v>64.75</v>
+        <v>61.93</v>
       </c>
     </row>
     <row r="3">
@@ -614,22 +614,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
         <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="G3" t="n">
-        <v>25.35</v>
+        <v>27.6</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -638,40 +638,40 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>3.75</v>
+        <v>3.449</v>
       </c>
       <c r="K3" t="n">
-        <v>0.211</v>
+        <v>0.161</v>
       </c>
       <c r="L3" t="n">
-        <v>10</v>
+        <v>48.89</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>15.56</v>
       </c>
       <c r="N3" t="n">
         <v>100</v>
       </c>
       <c r="O3" t="n">
-        <v>30</v>
+        <v>42.22</v>
       </c>
       <c r="P3" t="n">
-        <v>0.7</v>
+        <v>0.42</v>
       </c>
       <c r="Q3" t="n">
         <v>40</v>
       </c>
       <c r="R3" t="n">
-        <v>0.017</v>
+        <v>0.0101</v>
       </c>
       <c r="S3" t="n">
-        <v>10</v>
+        <v>2.22</v>
       </c>
       <c r="T3" t="n">
         <v>0.743</v>
       </c>
       <c r="U3" t="n">
-        <v>59.96</v>
+        <v>58.72</v>
       </c>
     </row>
     <row r="4">
@@ -681,22 +681,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
         <v>100</v>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="G4" t="n">
-        <v>24.31</v>
+        <v>35.92</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -705,40 +705,40 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.744</v>
+        <v>5.435</v>
       </c>
       <c r="K4" t="n">
-        <v>0.158</v>
+        <v>0.188</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>11.11</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>8.890000000000001</v>
       </c>
       <c r="N4" t="n">
         <v>100</v>
       </c>
       <c r="O4" t="n">
-        <v>60</v>
+        <v>37.78</v>
       </c>
       <c r="P4" t="n">
-        <v>0.3</v>
+        <v>0.76</v>
       </c>
       <c r="Q4" t="n">
-        <v>60</v>
+        <v>37.78</v>
       </c>
       <c r="R4" t="n">
-        <v>0.0103</v>
+        <v>0.0074</v>
       </c>
       <c r="S4" t="n">
-        <v>10</v>
+        <v>15.56</v>
       </c>
       <c r="T4" t="n">
-        <v>0.785</v>
+        <v>0.71</v>
       </c>
       <c r="U4" t="n">
-        <v>59.46</v>
+        <v>54.89</v>
       </c>
     </row>
     <row r="5">
@@ -748,22 +748,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
         <v>100</v>
       </c>
       <c r="F5" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="G5" t="n">
-        <v>35.27</v>
+        <v>38.12</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -772,40 +772,40 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>6.225</v>
+        <v>5.229</v>
       </c>
       <c r="K5" t="n">
-        <v>0.255</v>
+        <v>0.167</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>44.44</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>26.67</v>
       </c>
       <c r="N5" t="n">
         <v>100</v>
       </c>
       <c r="O5" t="n">
-        <v>30</v>
+        <v>42.22</v>
       </c>
       <c r="P5" t="n">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q5" t="n">
-        <v>30</v>
+        <v>37.78</v>
       </c>
       <c r="R5" t="n">
-        <v>0.008200000000000001</v>
+        <v>0.0055</v>
       </c>
       <c r="S5" t="n">
-        <v>10</v>
+        <v>6.67</v>
       </c>
       <c r="T5" t="n">
-        <v>0.785</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="U5" t="n">
-        <v>51.08</v>
+        <v>54.33</v>
       </c>
     </row>
     <row r="6">
@@ -815,22 +815,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
         <v>100</v>
       </c>
       <c r="F6" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="G6" t="n">
-        <v>26.27</v>
+        <v>35.5</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -839,65 +839,65 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.381</v>
+        <v>0.378</v>
       </c>
       <c r="K6" t="n">
-        <v>0.163</v>
+        <v>0.114</v>
       </c>
       <c r="L6" t="n">
-        <v>40</v>
+        <v>13.33</v>
       </c>
       <c r="M6" t="n">
-        <v>10</v>
+        <v>2.22</v>
       </c>
       <c r="N6" t="n">
-        <v>100</v>
+        <v>97.78</v>
       </c>
       <c r="O6" t="n">
-        <v>60</v>
+        <v>48.89</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="Q6" t="n">
-        <v>60</v>
+        <v>46.67</v>
       </c>
       <c r="R6" t="n">
-        <v>0</v>
+        <v>0.0108</v>
       </c>
       <c r="S6" t="n">
-        <v>20</v>
+        <v>2.22</v>
       </c>
       <c r="T6" t="n">
-        <v>0.785</v>
+        <v>0.71</v>
       </c>
       <c r="U6" t="n">
-        <v>40.12</v>
+        <v>52.59</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>blooms_taxonomy</t>
+          <t>misconceptions</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>100</v>
+        <v>33.33</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G7" t="n">
-        <v>26.94</v>
+        <v>31.02</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -906,13 +906,13 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>5.375</v>
+        <v>5.879</v>
       </c>
       <c r="K7" t="n">
-        <v>0.207</v>
+        <v>0.173</v>
       </c>
       <c r="L7" t="n">
-        <v>10</v>
+        <v>6.67</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -921,50 +921,50 @@
         <v>100</v>
       </c>
       <c r="O7" t="n">
-        <v>40</v>
+        <v>26.67</v>
       </c>
       <c r="P7" t="n">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="Q7" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="R7" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.0042</v>
       </c>
       <c r="S7" t="n">
-        <v>30</v>
+        <v>6.67</v>
       </c>
       <c r="T7" t="n">
-        <v>0.88</v>
+        <v>0.519</v>
       </c>
       <c r="U7" t="n">
-        <v>38.82</v>
+        <v>35.61</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>misconceptions</t>
+          <t>verbose</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" t="n">
         <v>100</v>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="G8" t="n">
-        <v>26.43</v>
+        <v>33.07</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -973,40 +973,40 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>5.431</v>
+        <v>2.856</v>
       </c>
       <c r="K8" t="n">
-        <v>0.207</v>
+        <v>0.176</v>
       </c>
       <c r="L8" t="n">
-        <v>20</v>
+        <v>11.11</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>4.44</v>
       </c>
       <c r="N8" t="n">
-        <v>100</v>
+        <v>97.78</v>
       </c>
       <c r="O8" t="n">
-        <v>30</v>
+        <v>26.67</v>
       </c>
       <c r="P8" t="n">
-        <v>0.5</v>
+        <v>0.31</v>
       </c>
       <c r="Q8" t="n">
-        <v>40</v>
+        <v>24.44</v>
       </c>
       <c r="R8" t="n">
-        <v>0.0018</v>
+        <v>0.0041</v>
       </c>
       <c r="S8" t="n">
-        <v>0</v>
+        <v>22.22</v>
       </c>
       <c r="T8" t="n">
-        <v>0.785</v>
+        <v>0.864</v>
       </c>
       <c r="U8" t="n">
-        <v>37.58</v>
+        <v>35.18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>